<commit_message>
Nueva etapa de filtrado
</commit_message>
<xml_diff>
--- a/Control_de_ruido/Textos_guia/BOM_Cancelador.xlsx
+++ b/Control_de_ruido/Textos_guia/BOM_Cancelador.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sfmer\OneDrive - Universidad Sergio Arboleda\Documentos\Sergio_Arboleda\SEMESTRE_8\Diseño_Producto_1\Producto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sfmer\OneDrive - Universidad Sergio Arboleda\Documentos\Sergio_Arboleda\SEMESTRE_8\Diseño_Producto_1\Producto\Cancelador_de_ruido\Control_de_ruido\Textos_guia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A33EFD-DC74-48E5-9890-12269D3B061E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF69D92B-7929-4228-9C2D-0056A02CA797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{19D0D2C8-7E19-472F-8F6A-EE8E802C78E3}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Resistencias</t>
   </si>
@@ -113,49 +113,61 @@
     <t>D4, D5</t>
   </si>
   <si>
-    <t>R0805 10M Ohm - Sigma Electrónica (sigmaelectronica.net)</t>
-  </si>
-  <si>
-    <t>R5, R7, R8</t>
-  </si>
-  <si>
     <t>R3, R6</t>
   </si>
   <si>
-    <t>R1, R2, R13, R14</t>
-  </si>
-  <si>
     <t>Falta que andres haga el amplificador</t>
   </si>
   <si>
-    <t>R10, R11, R12</t>
-  </si>
-  <si>
-    <t>https://www.sigmaelectronica.net/producto/r0805-10-ohmio/</t>
-  </si>
-  <si>
-    <t>C5, C6, C7</t>
-  </si>
-  <si>
-    <t>https://co.mouser.com/ProductDetail/Murata-Electronics/GRM188R71A225KE15D?qs=sGAEpiMZZMsh%252B1woXyUXj4CB84%2Fbv4tdJQymsS%252B5%252Byk%3D</t>
-  </si>
-  <si>
     <t>LD106D107MAB2A Kyocera AVX | Mouser Colombia</t>
   </si>
   <si>
-    <t>16SVPG220M Panasonic | Mouser Colombia</t>
-  </si>
-  <si>
     <t>C3, C4</t>
   </si>
   <si>
-    <t>1812CC104KAZ1A Kyocera AVX | Mouser Colombia</t>
-  </si>
-  <si>
     <t>L2, L3, L4</t>
   </si>
   <si>
     <t>TARJETA DE DESARROLLO ESP32-WROOM-32U (mactronica.com.co)</t>
+  </si>
+  <si>
+    <t>R1, R2, R16, R17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.sigmaelectronica.net/producto/r0805-10k/ </t>
+  </si>
+  <si>
+    <t>R5, R7, R8, R11,  R12, R14</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistencias 13 KOHM SMD 0805 1/8W 5% x10 (vistronica.com) </t>
+  </si>
+  <si>
+    <t>https://www.vistronica.com/componentes-pasivos/resistencias/TrimmerVerticalde500KOhm-detail.html</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R0805 100 OHM - Sigma Electrónica (sigmaelectronica.net) </t>
+  </si>
+  <si>
+    <t>CC0805 1NF 50V - Sigma Electrónica (sigmaelectronica.net)</t>
+  </si>
+  <si>
+    <t>C5, C6</t>
+  </si>
+  <si>
+    <t>https://www.sigmaelectronica.net/producto/cc0805-0-1uf50/</t>
+  </si>
+  <si>
+    <t>https://www.sigmaelectronica.net/producto/cond-220uf-16v/</t>
   </si>
 </sst>
 </file>
@@ -222,7 +234,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -274,10 +286,107 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
@@ -287,24 +396,69 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -313,84 +467,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -401,29 +501,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -741,15 +854,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA50067E-79DC-44FD-9163-85109DF1C1A7}">
   <dimension ref="C3:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="92.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="99" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="59.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="163.85546875" bestFit="1" customWidth="1"/>
@@ -757,158 +870,175 @@
   <sheetData>
     <row r="3" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="F4" s="9" t="s">
+      <c r="D4" s="17"/>
+      <c r="F4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="10"/>
-      <c r="I4" s="9" t="s">
+      <c r="G4" s="14"/>
+      <c r="I4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="10"/>
+      <c r="J4" s="14"/>
     </row>
     <row r="5" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C5" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="5" t="s">
+      <c r="C5" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="5" t="s">
-        <v>35</v>
+      <c r="J5" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C6" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="C6" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="5" t="s">
         <v>4</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="5" t="s">
         <v>7</v>
       </c>
       <c r="J6" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C9" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9" s="15"/>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C10" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="21" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="I7" s="7" t="s">
+    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C11" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I8" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>32</v>
+    </row>
+    <row r="12" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="10"/>
-      <c r="F22" s="9" t="s">
+      <c r="D22" s="14"/>
+      <c r="F22" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G22" s="10"/>
-      <c r="I22" s="9" t="s">
+      <c r="G22" s="14"/>
+      <c r="I22" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="J22" s="10"/>
+      <c r="J22" s="14"/>
     </row>
     <row r="23" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="15" t="s">
+      <c r="F23" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G23" s="14" t="s">
+      <c r="G23" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="I23" s="6" t="s">
+      <c r="I23" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J23" s="17"/>
+      <c r="J23" s="12"/>
     </row>
     <row r="24" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="11"/>
-      <c r="I24" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="J24" s="16"/>
+      <c r="D24" s="6"/>
+      <c r="I24" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J24" s="11"/>
     </row>
     <row r="25" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="12" t="s">
-        <v>40</v>
+      <c r="D25" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -930,15 +1060,17 @@
     <hyperlink ref="G6" r:id="rId6" display="https://co.mouser.com/ProductDetail/onsemi-Fairchild/SS34?qs=2ONuHmP%2FXzb3ub11UdFfdQ%3D%3D" xr:uid="{B0820D0A-511F-45E9-A2C8-A0E84FE8E708}"/>
     <hyperlink ref="G5" r:id="rId7" display="https://www.sigmaelectronica.net/producto/led-0805-verde/" xr:uid="{B7F0174F-855F-4A97-A36B-9E36CC22B383}"/>
     <hyperlink ref="G7" r:id="rId8" xr:uid="{780A5BC9-F716-4459-88B8-46B0D9B40C8A}"/>
-    <hyperlink ref="D8" r:id="rId9" display="https://www.sigmaelectronica.net/producto/r0805-10m-ohm/" xr:uid="{6F293908-29F5-49CD-92D0-4E8788B02C26}"/>
-    <hyperlink ref="D10" r:id="rId10" xr:uid="{61294E03-8D91-4ED3-AF32-F5C30AC66D23}"/>
-    <hyperlink ref="J8" r:id="rId11" xr:uid="{67A21DD2-E95C-496E-838B-80B26059BEC8}"/>
+    <hyperlink ref="D8" r:id="rId9" xr:uid="{6F293908-29F5-49CD-92D0-4E8788B02C26}"/>
+    <hyperlink ref="D11" r:id="rId10" xr:uid="{61294E03-8D91-4ED3-AF32-F5C30AC66D23}"/>
+    <hyperlink ref="J8" r:id="rId11" display="https://co.mouser.com/ProductDetail/Murata-Electronics/GRM188R71A225KE15D?qs=sGAEpiMZZMsh%252B1woXyUXj4CB84%2Fbv4tdJQymsS%252B5%252Byk%3D" xr:uid="{67A21DD2-E95C-496E-838B-80B26059BEC8}"/>
     <hyperlink ref="J5" r:id="rId12" display="https://co.mouser.com/ProductDetail/Kyocera-AVX/LD106D107MAB2A?qs=sGAEpiMZZMt7gvpyg0xT8h%252BpvM4D2LMciJXrgrFhEO4%3D" xr:uid="{BF094EC8-4443-4C2A-9B6D-F3305ABC5850}"/>
-    <hyperlink ref="J6" r:id="rId13" display="https://co.mouser.com/ProductDetail/Panasonic/16SVPG220M?qs=sGAEpiMZZMsh%252B1woXyUXjzWuff7xO%252BNrJKZJr8aXu90%3D" xr:uid="{10C54BED-8AE1-4274-B8FA-94CD2E35AE2C}"/>
-    <hyperlink ref="J7" r:id="rId14" display="https://co.mouser.com/ProductDetail/Kyocera-AVX/1812CC104KAZ1A?qs=lpAV6hZbGAs%252BH%2FFRM%252BS4kw%3D%3D" xr:uid="{C7A6B5D0-4A17-4F4C-97A3-6D87143A73F4}"/>
+    <hyperlink ref="J6" r:id="rId13" xr:uid="{10C54BED-8AE1-4274-B8FA-94CD2E35AE2C}"/>
+    <hyperlink ref="J7" r:id="rId14" xr:uid="{C7A6B5D0-4A17-4F4C-97A3-6D87143A73F4}"/>
     <hyperlink ref="D25" r:id="rId15" display="https://www.mactronica.com.co/tarjeta-de-desarrollo-esp32-wroom-32u" xr:uid="{824C4C31-6DA9-4485-B0D8-E259D2162032}"/>
+    <hyperlink ref="D10" r:id="rId16" display="https://www.vistronica.com/componentes-pasivos/resistencias/resistencias-13-kohm-smd-0805-18w-5-x10-detail.html" xr:uid="{1D1A5B17-6A38-40A7-BA9E-890D847E78A7}"/>
+    <hyperlink ref="D12" r:id="rId17" display="https://www.sigmaelectronica.net/producto/r0805-100-ohm/" xr:uid="{C3B552A6-795B-404D-86EF-0ACA166C1F52}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId16"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
se cambia esquematico por el realizo en proteus el 4/04, se cambian las huellas y se sube a PCB
</commit_message>
<xml_diff>
--- a/Control_de_ruido/Textos_guia/BOM_Cancelador.xlsx
+++ b/Control_de_ruido/Textos_guia/BOM_Cancelador.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sfmer\OneDrive - Universidad Sergio Arboleda\Documentos\Sergio_Arboleda\SEMESTRE_8\Diseño_Producto_1\Producto\Cancelador_de_ruido\Control_de_ruido\Textos_guia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\57318\Documents\Universidad\Semestre 8\Diseño de producto\Git_Hub\Cancelador_de_ruido\Control_de_ruido\Textos_guia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF69D92B-7929-4228-9C2D-0056A02CA797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC0B49D-E4EA-440D-BF1A-8B3625586700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{19D0D2C8-7E19-472F-8F6A-EE8E802C78E3}"/>
   </bookViews>
@@ -515,19 +515,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
@@ -537,6 +525,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -854,8 +854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA50067E-79DC-44FD-9163-85109DF1C1A7}">
   <dimension ref="C3:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -870,24 +870,24 @@
   <sheetData>
     <row r="3" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="F4" s="13" t="s">
+      <c r="D4" s="24"/>
+      <c r="F4" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="14"/>
-      <c r="I4" s="13" t="s">
+      <c r="G4" s="26"/>
+      <c r="I4" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="14"/>
+      <c r="J4" s="26"/>
     </row>
     <row r="5" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="15" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="4" t="s">
@@ -904,10 +904,10 @@
       </c>
     </row>
     <row r="6" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="17" t="s">
         <v>18</v>
       </c>
       <c r="F6" s="5" t="s">
@@ -924,10 +924,10 @@
       </c>
     </row>
     <row r="7" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="17" t="s">
         <v>19</v>
       </c>
       <c r="F7" s="8" t="s">
@@ -944,10 +944,10 @@
       </c>
     </row>
     <row r="8" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="17" t="s">
         <v>33</v>
       </c>
       <c r="I8" s="8" t="s">
@@ -958,32 +958,32 @@
       </c>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="J9" s="15"/>
+      <c r="J9" s="13"/>
     </row>
     <row r="10" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="17" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="11" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="21" t="s">
+      <c r="D11" s="17" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="12" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="22" t="s">
         <v>39</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -992,18 +992,18 @@
     </row>
     <row r="21" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="14"/>
-      <c r="F22" s="13" t="s">
+      <c r="D22" s="26"/>
+      <c r="F22" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="G22" s="14"/>
-      <c r="I22" s="13" t="s">
+      <c r="G22" s="26"/>
+      <c r="I22" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="J22" s="14"/>
+      <c r="J22" s="26"/>
     </row>
     <row r="23" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C23" s="4" t="s">

</xml_diff>